<commit_message>
Résultats par états fonctionnels
</commit_message>
<xml_diff>
--- a/src/loader_package/big_pre_load.xlsx
+++ b/src/loader_package/big_pre_load.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://poce-my.sharepoint.com/personal/charles_perold_edu_ece_fr/Documents/ING 3/Informatique - Java/_Projet Gui S5/_Projet GUI_Fork/java_project_desautel_pellen_perold/src/loader_package/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\java_project_desautel_pellen_perold\src\loader_package\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{2A97B4EA-A192-43BB-9E09-B9A2939F16BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3BC19E71-265D-4A4B-A135-39D7141E2354}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03CD7B1-1DBE-4ADD-850C-B0D3A5D792E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="elector" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5081" uniqueCount="1966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5081" uniqueCount="1917">
   <si>
     <t>Charles</t>
   </si>
@@ -5764,156 +5764,6 @@
     <t>kim</t>
   </si>
   <si>
-    <t> Alabama</t>
-  </si>
-  <si>
-    <t> Alaska</t>
-  </si>
-  <si>
-    <t> Arizona</t>
-  </si>
-  <si>
-    <t> Arkansas</t>
-  </si>
-  <si>
-    <t> California</t>
-  </si>
-  <si>
-    <t> Colorado</t>
-  </si>
-  <si>
-    <t> Connecticut</t>
-  </si>
-  <si>
-    <t> Delaware</t>
-  </si>
-  <si>
-    <t> Florida</t>
-  </si>
-  <si>
-    <t> Georgia</t>
-  </si>
-  <si>
-    <t> Hawaii</t>
-  </si>
-  <si>
-    <t> Idaho</t>
-  </si>
-  <si>
-    <t> Illinois</t>
-  </si>
-  <si>
-    <t> Indiana</t>
-  </si>
-  <si>
-    <t> Iowa</t>
-  </si>
-  <si>
-    <t> Kansas</t>
-  </si>
-  <si>
-    <t> Louisiana</t>
-  </si>
-  <si>
-    <t> Maine</t>
-  </si>
-  <si>
-    <t> Maryland</t>
-  </si>
-  <si>
-    <t> Michigan</t>
-  </si>
-  <si>
-    <t> Minnesota</t>
-  </si>
-  <si>
-    <t> Mississippi</t>
-  </si>
-  <si>
-    <t> Missouri</t>
-  </si>
-  <si>
-    <t> Montana</t>
-  </si>
-  <si>
-    <t> Nebraska</t>
-  </si>
-  <si>
-    <t> Nevada</t>
-  </si>
-  <si>
-    <t> New Hampshire</t>
-  </si>
-  <si>
-    <t> New Jersey</t>
-  </si>
-  <si>
-    <t> New Mexico</t>
-  </si>
-  <si>
-    <t> New York</t>
-  </si>
-  <si>
-    <t> North Carolina</t>
-  </si>
-  <si>
-    <t> North Dakota</t>
-  </si>
-  <si>
-    <t> Ohio</t>
-  </si>
-  <si>
-    <t> Oklahoma</t>
-  </si>
-  <si>
-    <t> Oregon</t>
-  </si>
-  <si>
-    <t> Rhode Island</t>
-  </si>
-  <si>
-    <t> South Carolina</t>
-  </si>
-  <si>
-    <t> South Dakota</t>
-  </si>
-  <si>
-    <t> Tennessee</t>
-  </si>
-  <si>
-    <t> Texas</t>
-  </si>
-  <si>
-    <t> Utah</t>
-  </si>
-  <si>
-    <t> Vermont</t>
-  </si>
-  <si>
-    <t> Washington</t>
-  </si>
-  <si>
-    <t> West Virginia</t>
-  </si>
-  <si>
-    <t> Wisconsin</t>
-  </si>
-  <si>
-    <t> Wyoming</t>
-  </si>
-  <si>
-    <t> Kentucky</t>
-  </si>
-  <si>
-    <t> Massachusetts</t>
-  </si>
-  <si>
-    <t> Pennsylvania</t>
-  </si>
-  <si>
-    <t> Virginia</t>
-  </si>
-  <si>
     <t>Clementine</t>
   </si>
   <si>
@@ -5936,6 +5786,9 @@
   </si>
   <si>
     <t>CHARLIE</t>
+  </si>
+  <si>
+    <t>Rhode Island</t>
   </si>
 </sst>
 </file>
@@ -6287,8 +6140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6303,19 +6156,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1960</v>
+        <v>1910</v>
       </c>
       <c r="B1" t="s">
-        <v>1961</v>
+        <v>1911</v>
       </c>
       <c r="C1" t="s">
-        <v>1962</v>
+        <v>1912</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -6375,7 +6228,7 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -6495,7 +6348,7 @@
         <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -6563,7 +6416,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1964</v>
+        <v>1914</v>
       </c>
       <c r="B14" t="s">
         <v>62</v>
@@ -6583,7 +6436,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1965</v>
+        <v>1915</v>
       </c>
       <c r="B15" t="s">
         <v>65</v>
@@ -6595,7 +6448,7 @@
         <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -6715,7 +6568,7 @@
         <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -7235,7 +7088,7 @@
         <v>134</v>
       </c>
       <c r="E47" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -7655,7 +7508,7 @@
         <v>6</v>
       </c>
       <c r="E68" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -8135,7 +7988,7 @@
         <v>48</v>
       </c>
       <c r="E92" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F92">
         <v>0</v>
@@ -8575,7 +8428,7 @@
         <v>20</v>
       </c>
       <c r="E114" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F114">
         <v>0</v>
@@ -8995,7 +8848,7 @@
         <v>81</v>
       </c>
       <c r="E135" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F135">
         <v>0</v>
@@ -9475,7 +9328,7 @@
         <v>386</v>
       </c>
       <c r="E159" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F159">
         <v>0</v>
@@ -9775,7 +9628,7 @@
         <v>20</v>
       </c>
       <c r="E174" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F174">
         <v>0</v>
@@ -10315,7 +10168,7 @@
         <v>1</v>
       </c>
       <c r="E201" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F201">
         <v>0</v>
@@ -10795,7 +10648,7 @@
         <v>64</v>
       </c>
       <c r="E225" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F225">
         <v>0</v>
@@ -11215,7 +11068,7 @@
         <v>56</v>
       </c>
       <c r="E246" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F246">
         <v>0</v>
@@ -11455,7 +11308,7 @@
         <v>726</v>
       </c>
       <c r="E258" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F258">
         <v>0</v>
@@ -11695,7 +11548,7 @@
         <v>293</v>
       </c>
       <c r="E270" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F270">
         <v>0</v>
@@ -11875,7 +11728,7 @@
         <v>81</v>
       </c>
       <c r="E279" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F279">
         <v>0</v>
@@ -12115,7 +11968,7 @@
         <v>720</v>
       </c>
       <c r="E291" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F291">
         <v>0</v>
@@ -12355,7 +12208,7 @@
         <v>189</v>
       </c>
       <c r="E303" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F303">
         <v>0</v>
@@ -12595,7 +12448,7 @@
         <v>56</v>
       </c>
       <c r="E315" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F315">
         <v>0</v>
@@ -12895,7 +12748,7 @@
         <v>48</v>
       </c>
       <c r="E330" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F330">
         <v>0</v>
@@ -13135,7 +12988,7 @@
         <v>100</v>
       </c>
       <c r="E342" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F342">
         <v>0</v>
@@ -13315,7 +13168,7 @@
         <v>113</v>
       </c>
       <c r="E351" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F351">
         <v>0</v>
@@ -13675,7 +13528,7 @@
         <v>39</v>
       </c>
       <c r="E369" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F369">
         <v>0</v>
@@ -13855,7 +13708,7 @@
         <v>39</v>
       </c>
       <c r="E378" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F378">
         <v>0</v>
@@ -14095,7 +13948,7 @@
         <v>100</v>
       </c>
       <c r="E390" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F390">
         <v>0</v>
@@ -14395,7 +14248,7 @@
         <v>419</v>
       </c>
       <c r="E405" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F405">
         <v>0</v>
@@ -14635,7 +14488,7 @@
         <v>1</v>
       </c>
       <c r="E417" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F417">
         <v>0</v>
@@ -14875,7 +14728,7 @@
         <v>350</v>
       </c>
       <c r="E429" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F429">
         <v>0</v>
@@ -15055,7 +14908,7 @@
         <v>72</v>
       </c>
       <c r="E438" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F438">
         <v>0</v>
@@ -15355,7 +15208,7 @@
         <v>134</v>
       </c>
       <c r="E453" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F453">
         <v>0</v>
@@ -15655,7 +15508,7 @@
         <v>64</v>
       </c>
       <c r="E468" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F468">
         <v>0</v>
@@ -16015,7 +15868,7 @@
         <v>113</v>
       </c>
       <c r="E486" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F486">
         <v>0</v>
@@ -16315,7 +16168,7 @@
         <v>121</v>
       </c>
       <c r="E501" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F501">
         <v>0</v>
@@ -16675,7 +16528,7 @@
         <v>720</v>
       </c>
       <c r="E519" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F519">
         <v>0</v>
@@ -17035,7 +16888,7 @@
         <v>189</v>
       </c>
       <c r="E537" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F537">
         <v>0</v>
@@ -17395,7 +17248,7 @@
         <v>155</v>
       </c>
       <c r="E555" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F555">
         <v>0</v>
@@ -17695,7 +17548,7 @@
         <v>165</v>
       </c>
       <c r="E570" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F570">
         <v>0</v>
@@ -18175,7 +18028,7 @@
         <v>350</v>
       </c>
       <c r="E594" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F594">
         <v>0</v>
@@ -18535,7 +18388,7 @@
         <v>56</v>
       </c>
       <c r="E612" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F612">
         <v>0</v>
@@ -18895,7 +18748,7 @@
         <v>117</v>
       </c>
       <c r="E630" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F630">
         <v>0</v>
@@ -19255,7 +19108,7 @@
         <v>254</v>
       </c>
       <c r="E648" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F648">
         <v>0</v>
@@ -19735,7 +19588,7 @@
         <v>81</v>
       </c>
       <c r="E672" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F672">
         <v>0</v>
@@ -20215,7 +20068,7 @@
         <v>343</v>
       </c>
       <c r="E696" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F696">
         <v>0</v>
@@ -20695,7 +20548,7 @@
         <v>100</v>
       </c>
       <c r="E720" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F720">
         <v>0</v>
@@ -21115,7 +20968,7 @@
         <v>64</v>
       </c>
       <c r="E741" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F741">
         <v>0</v>
@@ -21655,7 +21508,7 @@
         <v>56</v>
       </c>
       <c r="E768" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F768">
         <v>0</v>
@@ -22255,7 +22108,7 @@
         <v>293</v>
       </c>
       <c r="E798" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F798">
         <v>0</v>
@@ -22555,7 +22408,7 @@
         <v>350</v>
       </c>
       <c r="E813" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F813">
         <v>0</v>
@@ -22855,7 +22708,7 @@
         <v>20</v>
       </c>
       <c r="E828" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F828">
         <v>0</v>
@@ -23095,7 +22948,7 @@
         <v>117</v>
       </c>
       <c r="E840" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F840">
         <v>0</v>
@@ -23335,7 +23188,7 @@
         <v>599</v>
       </c>
       <c r="E852" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F852">
         <v>0</v>
@@ -23575,7 +23428,7 @@
         <v>35</v>
       </c>
       <c r="E864" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F864">
         <v>0</v>
@@ -23815,7 +23668,7 @@
         <v>4</v>
       </c>
       <c r="E876" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F876">
         <v>0</v>
@@ -23995,7 +23848,7 @@
         <v>368</v>
       </c>
       <c r="E885" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F885">
         <v>0</v>
@@ -24175,7 +24028,7 @@
         <v>840</v>
       </c>
       <c r="E894" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F894">
         <v>0</v>
@@ -24415,7 +24268,7 @@
         <v>155</v>
       </c>
       <c r="E906" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F906">
         <v>0</v>
@@ -24595,7 +24448,7 @@
         <v>77</v>
       </c>
       <c r="E915" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F915">
         <v>0</v>
@@ -24855,7 +24708,7 @@
         <v>720</v>
       </c>
       <c r="E928" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F928">
         <v>0</v>
@@ -25175,7 +25028,7 @@
         <v>6</v>
       </c>
       <c r="E944" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F944">
         <v>0</v>
@@ -25715,7 +25568,7 @@
         <v>100</v>
       </c>
       <c r="E971" t="s">
-        <v>1963</v>
+        <v>1913</v>
       </c>
       <c r="F971">
         <v>0</v>
@@ -26443,8 +26296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1851D91F-DA7C-4EA5-959B-DCDBAE8FBF58}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26456,7 +26309,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1908</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1">
         <v>10</v>
@@ -26470,7 +26323,7 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>1909</v>
+        <v>67</v>
       </c>
       <c r="B2" s="5">
         <v>10</v>
@@ -26484,7 +26337,7 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1910</v>
+        <v>64</v>
       </c>
       <c r="B3" s="5">
         <v>10</v>
@@ -26498,7 +26351,7 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>1911</v>
+        <v>134</v>
       </c>
       <c r="B4" s="5">
         <v>10</v>
@@ -26512,7 +26365,7 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>1912</v>
+        <v>27</v>
       </c>
       <c r="B5" s="5">
         <v>10</v>
@@ -26526,7 +26379,7 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>1913</v>
+        <v>368</v>
       </c>
       <c r="B6" s="5">
         <v>10</v>
@@ -26540,7 +26393,7 @@
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>1914</v>
+        <v>173</v>
       </c>
       <c r="B7" s="5">
         <v>10</v>
@@ -26554,7 +26407,7 @@
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>1915</v>
+        <v>72</v>
       </c>
       <c r="B8" s="5">
         <v>10</v>
@@ -26568,7 +26421,7 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>1916</v>
+        <v>182</v>
       </c>
       <c r="B9" s="5">
         <v>10</v>
@@ -26582,7 +26435,7 @@
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>1917</v>
+        <v>31</v>
       </c>
       <c r="B10" s="5">
         <v>10</v>
@@ -26596,7 +26449,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>1918</v>
+        <v>293</v>
       </c>
       <c r="B11" s="5">
         <v>10</v>
@@ -26610,7 +26463,7 @@
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>1919</v>
+        <v>87</v>
       </c>
       <c r="B12" s="5">
         <v>10</v>
@@ -26624,7 +26477,7 @@
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>1920</v>
+        <v>81</v>
       </c>
       <c r="B13" s="5">
         <v>10</v>
@@ -26638,7 +26491,7 @@
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>1921</v>
+        <v>303</v>
       </c>
       <c r="B14" s="5">
         <v>10</v>
@@ -26652,7 +26505,7 @@
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>1922</v>
+        <v>52</v>
       </c>
       <c r="B15" s="5">
         <v>10</v>
@@ -26666,7 +26519,7 @@
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>1923</v>
+        <v>56</v>
       </c>
       <c r="B16" s="5">
         <v>10</v>
@@ -26680,7 +26533,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>1954</v>
+        <v>43</v>
       </c>
       <c r="B17" s="5">
         <v>10</v>
@@ -26694,7 +26547,7 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>1924</v>
+        <v>169</v>
       </c>
       <c r="B18" s="5">
         <v>10</v>
@@ -26708,7 +26561,7 @@
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>1925</v>
+        <v>189</v>
       </c>
       <c r="B19" s="5">
         <v>10</v>
@@ -26722,7 +26575,7 @@
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>1926</v>
+        <v>443</v>
       </c>
       <c r="B20" s="5">
         <v>10</v>
@@ -26736,7 +26589,7 @@
     </row>
     <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>1955</v>
+        <v>350</v>
       </c>
       <c r="B21" s="5">
         <v>10</v>
@@ -26750,7 +26603,7 @@
     </row>
     <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>1927</v>
+        <v>4</v>
       </c>
       <c r="B22" s="5">
         <v>10</v>
@@ -26764,7 +26617,7 @@
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>1928</v>
+        <v>343</v>
       </c>
       <c r="B23" s="5">
         <v>10</v>
@@ -26778,7 +26631,7 @@
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>1929</v>
+        <v>599</v>
       </c>
       <c r="B24" s="5">
         <v>10</v>
@@ -26792,7 +26645,7 @@
     </row>
     <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>1930</v>
+        <v>20</v>
       </c>
       <c r="B25" s="5">
         <v>10</v>
@@ -26806,7 +26659,7 @@
     </row>
     <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>1931</v>
+        <v>60</v>
       </c>
       <c r="B26" s="5">
         <v>10</v>
@@ -26820,7 +26673,7 @@
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>1932</v>
+        <v>100</v>
       </c>
       <c r="B27" s="5">
         <v>10</v>
@@ -26834,7 +26687,7 @@
     </row>
     <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>1933</v>
+        <v>155</v>
       </c>
       <c r="B28" s="5">
         <v>10</v>
@@ -26848,7 +26701,7 @@
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>1934</v>
+        <v>16</v>
       </c>
       <c r="B29" s="5">
         <v>10</v>
@@ -26862,7 +26715,7 @@
     </row>
     <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>1935</v>
+        <v>419</v>
       </c>
       <c r="B30" s="5">
         <v>10</v>
@@ -26876,7 +26729,7 @@
     </row>
     <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>1936</v>
+        <v>720</v>
       </c>
       <c r="B31" s="5">
         <v>10</v>
@@ -26890,7 +26743,7 @@
     </row>
     <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>1937</v>
+        <v>840</v>
       </c>
       <c r="B32" s="5">
         <v>10</v>
@@ -26904,7 +26757,7 @@
     </row>
     <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>1938</v>
+        <v>141</v>
       </c>
       <c r="B33" s="5">
         <v>10</v>
@@ -26918,7 +26771,7 @@
     </row>
     <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>1939</v>
+        <v>97</v>
       </c>
       <c r="B34" s="5">
         <v>10</v>
@@ -26932,7 +26785,7 @@
     </row>
     <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>1940</v>
+        <v>39</v>
       </c>
       <c r="B35" s="5">
         <v>10</v>
@@ -26946,7 +26799,7 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>1941</v>
+        <v>145</v>
       </c>
       <c r="B36" s="5">
         <v>10</v>
@@ -26960,7 +26813,7 @@
     </row>
     <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>1942</v>
+        <v>113</v>
       </c>
       <c r="B37" s="5">
         <v>10</v>
@@ -26974,7 +26827,7 @@
     </row>
     <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>1956</v>
+        <v>121</v>
       </c>
       <c r="B38" s="5">
         <v>10</v>
@@ -26988,7 +26841,7 @@
     </row>
     <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>1943</v>
+        <v>1916</v>
       </c>
       <c r="B39" s="5">
         <v>10</v>
@@ -27002,7 +26855,7 @@
     </row>
     <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>1944</v>
+        <v>726</v>
       </c>
       <c r="B40" s="5">
         <v>10</v>
@@ -27016,7 +26869,7 @@
     </row>
     <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>1945</v>
+        <v>223</v>
       </c>
       <c r="B41" s="5">
         <v>10</v>
@@ -27030,7 +26883,7 @@
     </row>
     <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>1946</v>
+        <v>117</v>
       </c>
       <c r="B42" s="5">
         <v>10</v>
@@ -27044,7 +26897,7 @@
     </row>
     <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>1947</v>
+        <v>165</v>
       </c>
       <c r="B43" s="5">
         <v>10</v>
@@ -27058,7 +26911,7 @@
     </row>
     <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>1948</v>
+        <v>77</v>
       </c>
       <c r="B44" s="5">
         <v>10</v>
@@ -27072,7 +26925,7 @@
     </row>
     <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>1949</v>
+        <v>254</v>
       </c>
       <c r="B45" s="5">
         <v>10</v>
@@ -27086,7 +26939,7 @@
     </row>
     <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>1957</v>
+        <v>1</v>
       </c>
       <c r="B46" s="5">
         <v>10</v>
@@ -27100,7 +26953,7 @@
     </row>
     <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>1950</v>
+        <v>6</v>
       </c>
       <c r="B47" s="5">
         <v>10</v>
@@ -27114,7 +26967,7 @@
     </row>
     <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>1951</v>
+        <v>386</v>
       </c>
       <c r="B48" s="5">
         <v>10</v>
@@ -27128,7 +26981,7 @@
     </row>
     <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>1952</v>
+        <v>35</v>
       </c>
       <c r="B49" s="5">
         <v>10</v>
@@ -27142,7 +26995,7 @@
     </row>
     <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>1953</v>
+        <v>226</v>
       </c>
       <c r="B50" s="5">
         <v>10</v>
@@ -27188,10 +27041,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>1958</v>
+        <v>1908</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1959</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Start / Pause / End terminé
</commit_message>
<xml_diff>
--- a/src/loader_package/big_pre_load.xlsx
+++ b/src/loader_package/big_pre_load.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://poce-my.sharepoint.com/personal/charles_perold_edu_ece_fr/Documents/ING 3/Informatique - Java/_Projet Gui S5/_Projet GUI_Fork/java_project_desautel_pellen_perold/src/loader_package/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="114_{4560B6F7-C561-409F-9E40-3EAEB2945EBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CF054478-8325-4806-A1C4-3A74D51CE4A5}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="114_{4560B6F7-C561-409F-9E40-3EAEB2945EBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E82AF0E1-137D-4C63-A55A-3987235B9526}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="27977" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6149,7 +6149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D188" sqref="D188"/>
     </sheetView>
   </sheetViews>
@@ -26306,7 +26306,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -26509,7 +26509,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.9" x14ac:dyDescent="0.4">
@@ -26579,7 +26579,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.9" x14ac:dyDescent="0.4">
@@ -26677,7 +26677,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.9" x14ac:dyDescent="0.4">
@@ -26775,7 +26775,7 @@
         <v>1</v>
       </c>
       <c r="D33" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.9" x14ac:dyDescent="0.4">
@@ -26859,7 +26859,7 @@
         <v>1</v>
       </c>
       <c r="D39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.9" x14ac:dyDescent="0.4">
@@ -26929,7 +26929,7 @@
         <v>1</v>
       </c>
       <c r="D44" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.9" x14ac:dyDescent="0.4">
@@ -26985,7 +26985,7 @@
         <v>1</v>
       </c>
       <c r="D48" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.9" x14ac:dyDescent="0.4">
@@ -27013,7 +27013,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.4">

</xml_diff>